<commit_message>
Week 4 Workbook Update
</commit_message>
<xml_diff>
--- a/Dungeonmancer Workbook.xlsx
+++ b/Dungeonmancer Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Desktop\Capstone Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2250B0C-2473-4CB2-B9BA-FA70CBF7B9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE89F6D-BA5E-4B67-9298-5AA8473759AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{C7E3B102-2D79-404D-96C8-06FB473DFC22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{C7E3B102-2D79-404D-96C8-06FB473DFC22}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="123">
   <si>
     <t>Team Members</t>
   </si>
@@ -247,6 +247,171 @@
   </si>
   <si>
     <t>Users will be able to play D&amp;D live with their character sheet in the program, allowing them to perform ability checks and attack rolls right from the program.</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>Run Tutorial</t>
+  </si>
+  <si>
+    <t>The user will open the program for the first time and click through the tutorial steps.</t>
+  </si>
+  <si>
+    <t>Once all of the steps in the creation tutorial have appeared and the user is taken to the empty character manager afterwards</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>Run  without Tutorial</t>
+  </si>
+  <si>
+    <t>The user will open the program after having already completed the tutorial at a previous time and the tutorial will no longer appear.</t>
+  </si>
+  <si>
+    <t>Upon opening the application, the user is taken directly to the character manager screen</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>Walkthrough Character Creation</t>
+  </si>
+  <si>
+    <t>The user will fill out the pages of steps towards character creation in full</t>
+  </si>
+  <si>
+    <t>The user successfully creates a character and is taken to the character's page</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>Incomplete Character Creation</t>
+  </si>
+  <si>
+    <t>The user will leave a page on the character creation screen incomplete and attempt to continue</t>
+  </si>
+  <si>
+    <t>The user is alerted that the step is incomplete and must fill it out before continuing</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>Cancelled Character Creation</t>
+  </si>
+  <si>
+    <t>A player will prtially complete making a character then cancel the process</t>
+  </si>
+  <si>
+    <t>The user will be prompted on if they'd like to save a draft of their work or delete their progress, then be returned to the main menu</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>Opening Character Sheet</t>
+  </si>
+  <si>
+    <t>The user will select their character's name on a list</t>
+  </si>
+  <si>
+    <t>The character sheet of the character will be displayed</t>
+  </si>
+  <si>
+    <t>Interacting with Character Sheet</t>
+  </si>
+  <si>
+    <t>User will select a skill check on their character sheet that they'd like to make</t>
+  </si>
+  <si>
+    <t>A dice roll is completed, automatically adding the character's associated bonuses, and displaying the result</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>Changing a Character's Stats</t>
+  </si>
+  <si>
+    <t>The stat will change and all associated skills and bonuses will automatically update</t>
+  </si>
+  <si>
+    <t>A user will select the edit button on their character sheet and attempt to change one of their character's core stats</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>Play Mode Attack Roll</t>
+  </si>
+  <si>
+    <t>A user will attempt to make an attack roll from their character sheet</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>6B</t>
+  </si>
+  <si>
+    <t>6C</t>
+  </si>
+  <si>
+    <t>Creating a homebrew class</t>
+  </si>
+  <si>
+    <t>Creating a homebrew race</t>
+  </si>
+  <si>
+    <t>Creating a homebrew background</t>
+  </si>
+  <si>
+    <t>A user will attempt to create a homebrew class upon being prompted to choose one</t>
+  </si>
+  <si>
+    <t>An attack roll will be made, adding all the relevant bonuses automatically, and the result will be displayed</t>
+  </si>
+  <si>
+    <t>The user will be walked through the steps of creating a class and the option will be permanently added to the class selection list</t>
+  </si>
+  <si>
+    <t>A user will attempt to create a homebrew race upon being prompted to choose one</t>
+  </si>
+  <si>
+    <t>A user will attempt to create a homebrew background upon being prompted to choose one</t>
+  </si>
+  <si>
+    <t>The user will be walked through the steps of creating a race and the option will be permanently added to the race selection list</t>
+  </si>
+  <si>
+    <t>The user will be walked through the steps of creating a background and the option will be permanently added to the baclground selection list</t>
+  </si>
+  <si>
+    <t>10/29 and 10/31</t>
+  </si>
+  <si>
+    <t>An initial, early development stage of the UI was reached, found under Work Log 1 in Github</t>
+  </si>
+  <si>
+    <t>Navigation between the existing pages for character creation was completed and a feature to select classes was created</t>
+  </si>
+  <si>
+    <t>The Class and Race pages were completed without a homebrew option yet, though some design work may still need to be done on them later in development</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>The background page was completed code-wise, the only thing left on it is the descriptions to be written for each background</t>
+  </si>
+  <si>
+    <t>A way to save progress as the character is being created was achieved</t>
   </si>
 </sst>
 </file>
@@ -335,7 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -357,35 +522,32 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1284,19 +1446,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1305,23 +1467,23 @@
       <c r="B3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1345,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA97EAC-8F0B-44EB-A2B8-2DB696346B43}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1358,11 +1520,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1455,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DBC3CE-F62F-46C9-9C62-091213B3C912}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1465,22 +1627,21 @@
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="27.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="20" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1495,7 +1656,7 @@
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1516,7 +1677,7 @@
       <c r="D3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" s="5"/>
@@ -1537,7 +1698,7 @@
       <c r="D4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="5">
         <v>2</v>
       </c>
       <c r="F4" s="5">
@@ -1560,7 +1721,7 @@
       <c r="D5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1583,7 +1744,7 @@
       <c r="D6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1606,7 +1767,7 @@
       <c r="D7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="5">
         <v>2</v>
       </c>
       <c r="F7" s="5">
@@ -1629,7 +1790,7 @@
       <c r="D8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1652,7 +1813,7 @@
       <c r="D9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="5">
         <v>3</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1675,7 +1836,7 @@
       <c r="D10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="5">
         <v>3</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1698,7 +1859,7 @@
       <c r="D11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="5">
         <v>3</v>
       </c>
       <c r="F11" s="5">
@@ -1719,7 +1880,7 @@
       <c r="D12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="5">
         <v>3</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1734,7 +1895,7 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="18"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
@@ -1743,7 +1904,7 @@
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="18"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
@@ -1752,7 +1913,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="18"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
@@ -1761,7 +1922,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
@@ -1770,7 +1931,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
@@ -1779,7 +1940,7 @@
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
@@ -1788,7 +1949,7 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="18"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
@@ -1797,7 +1958,7 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
@@ -1806,7 +1967,7 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
@@ -1815,7 +1976,7 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="18"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
@@ -1824,7 +1985,7 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="18"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
@@ -1833,7 +1994,7 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="18"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
@@ -1842,7 +2003,7 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="18"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
@@ -1851,7 +2012,7 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="18"/>
+      <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
@@ -1860,7 +2021,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="18"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
@@ -1869,7 +2030,7 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="18"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
@@ -1878,7 +2039,7 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="18"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
@@ -1887,7 +2048,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="18"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
@@ -1896,7 +2057,7 @@
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="18"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
@@ -1905,7 +2066,7 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="18"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
@@ -1914,7 +2075,7 @@
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="18"/>
+      <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
@@ -1923,7 +2084,7 @@
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="18"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
@@ -1932,7 +2093,7 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="18"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
@@ -1941,7 +2102,7 @@
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="18"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
@@ -1950,7 +2111,7 @@
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="18"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
@@ -1959,7 +2120,7 @@
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="18"/>
+      <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
@@ -1968,7 +2129,7 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="18"/>
+      <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
@@ -1977,7 +2138,7 @@
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="18"/>
+      <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
@@ -1986,7 +2147,7 @@
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="18"/>
+      <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
@@ -1995,7 +2156,7 @@
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="18"/>
+      <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
@@ -2004,7 +2165,7 @@
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="18"/>
+      <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
@@ -2013,7 +2174,7 @@
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="18"/>
+      <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
@@ -2022,7 +2183,7 @@
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="18"/>
+      <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
@@ -2031,7 +2192,7 @@
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="18"/>
+      <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
@@ -2049,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E746FEB-1AF3-4B65-B309-347451BAB3BF}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F18"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,14 +2226,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2094,101 +2255,245 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>6</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -2235,8 +2540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBA459C-639D-4278-A20F-A9580A80CD7A}">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,45 +2574,105 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="10">
+        <v>45965</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="10">
+        <v>45968</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10">
+        <v>45974</v>
+      </c>
+      <c r="C5" s="5">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10">
+        <v>45981</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
@@ -3398,6 +3763,13 @@
       <c r="F142" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{BFA570D6-B151-4D48-B3B5-5BE1B03F7B37}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{38E37FBB-12DD-4F51-80A2-F845028CA25B}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{99B12195-7FD3-4458-8B31-CD283068C436}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{9BCBBEA7-43F1-4A96-BECC-4D817E8E3DAF}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{7EA218AC-316C-495F-9F9D-6761A0AB1923}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>